<commit_message>
* Attribute 'diffs' no longer influences result calculations. * Result limits are present in summary layout if they were specified. * Dumping the SAXException message once again as it is not always dumped by the Xerces parser.
</commit_message>
<xml_diff>
--- a/tests/data/desired/columnscomparisonreport.xlsx
+++ b/tests/data/desired/columnscomparisonreport.xlsx
@@ -22,18 +22,18 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="true">normal!$B$2:$I$10</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="true">detailed!$B$2:$G$26</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="true">aggregated!$B$2:$H$5</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="true">summary!$B$2:$D$10</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="true">summary!$B$2:$D$13</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="true">interlaced2!$B$2:$I$10</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="true">normal2!$B$2:$I$10</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="true">detailed2!$B$2:$G$26</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="8" hidden="true">aggregated2!$B$2:$H$5</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="9" hidden="true">summary2!$B$2:$D$10</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="9" hidden="true">summary2!$B$2:$D$13</definedName>
   </definedNames>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="402" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="408" uniqueCount="57">
   <si>
     <t># of Diffs</t>
   </si>
@@ -173,25 +173,34 @@
     <t>Abone8</t>
   </si>
   <si>
+    <t>Total Rows</t>
+  </si>
+  <si>
     <t>Equal Rows</t>
   </si>
   <si>
+    <t>Different Rows</t>
+  </si>
+  <si>
     <t>Matching Rows</t>
   </si>
   <si>
-    <t>Different Rows</t>
-  </si>
-  <si>
-    <t>Total Rows</t>
-  </si>
-  <si>
-    <t>(Source1) - Rows</t>
+    <t>Non-matching Rows</t>
+  </si>
+  <si>
+    <t>(Source1) - Total Rows</t>
+  </si>
+  <si>
+    <t>(Source1) - Matching Rows</t>
   </si>
   <si>
     <t>(Source1) - Non-matching Rows</t>
   </si>
   <si>
-    <t>(Source2) - Rows</t>
+    <t>(Source2) - Total Rows</t>
+  </si>
+  <si>
+    <t>(Source2) - Matching Rows</t>
   </si>
   <si>
     <t>(Source2) - Non-matching Rows</t>
@@ -578,10 +587,10 @@
         <v>46</v>
       </c>
       <c r="C3" t="n">
-        <v>2.0</v>
+        <v>8.0</v>
       </c>
       <c r="D3" t="n" s="6">
-        <v>0.25</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="4">
@@ -589,10 +598,10 @@
         <v>47</v>
       </c>
       <c r="C4" t="n">
-        <v>4.0</v>
+        <v>2.0</v>
       </c>
       <c r="D4" t="n" s="6">
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="5">
@@ -611,10 +620,10 @@
         <v>49</v>
       </c>
       <c r="C6" t="n">
-        <v>8.0</v>
+        <v>4.0</v>
       </c>
       <c r="D6" t="n" s="6">
-        <v>1.0</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="7">
@@ -622,10 +631,10 @@
         <v>50</v>
       </c>
       <c r="C7" t="n">
-        <v>6.0</v>
+        <v>4.0</v>
       </c>
       <c r="D7" t="n" s="6">
-        <v>0.75</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="8">
@@ -633,10 +642,10 @@
         <v>51</v>
       </c>
       <c r="C8" t="n">
-        <v>2.0</v>
+        <v>6.0</v>
       </c>
       <c r="D8" t="n" s="6">
-        <v>0.3333333333333333</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="9">
@@ -644,10 +653,10 @@
         <v>52</v>
       </c>
       <c r="C9" t="n">
-        <v>6.0</v>
+        <v>2.0</v>
       </c>
       <c r="D9" t="n" s="6">
-        <v>0.75</v>
+        <v>0.6666666666666666</v>
       </c>
     </row>
     <row r="10">
@@ -661,8 +670,41 @@
         <v>0.3333333333333333</v>
       </c>
     </row>
+    <row r="11">
+      <c r="B11" t="s" s="3">
+        <v>54</v>
+      </c>
+      <c r="C11" t="n">
+        <v>6.0</v>
+      </c>
+      <c r="D11" t="n" s="6">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="B12" t="s" s="3">
+        <v>55</v>
+      </c>
+      <c r="C12" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="D12" t="n" s="6">
+        <v>0.6666666666666666</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="B13" t="s" s="3">
+        <v>56</v>
+      </c>
+      <c r="C13" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="D13" t="n" s="6">
+        <v>0.3333333333333333</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="B2:D10"/>
+  <autoFilter ref="B2:D13"/>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
@@ -1549,10 +1591,10 @@
         <v>46</v>
       </c>
       <c r="C3" t="n">
-        <v>2.0</v>
+        <v>8.0</v>
       </c>
       <c r="D3" t="n" s="6">
-        <v>0.25</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="4">
@@ -1560,10 +1602,10 @@
         <v>47</v>
       </c>
       <c r="C4" t="n">
-        <v>4.0</v>
+        <v>2.0</v>
       </c>
       <c r="D4" t="n" s="6">
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="5">
@@ -1582,10 +1624,10 @@
         <v>49</v>
       </c>
       <c r="C6" t="n">
-        <v>8.0</v>
+        <v>4.0</v>
       </c>
       <c r="D6" t="n" s="6">
-        <v>1.0</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="7">
@@ -1593,10 +1635,10 @@
         <v>50</v>
       </c>
       <c r="C7" t="n">
-        <v>6.0</v>
+        <v>4.0</v>
       </c>
       <c r="D7" t="n" s="6">
-        <v>0.75</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="8">
@@ -1604,10 +1646,10 @@
         <v>51</v>
       </c>
       <c r="C8" t="n">
-        <v>2.0</v>
+        <v>6.0</v>
       </c>
       <c r="D8" t="n" s="6">
-        <v>0.3333333333333333</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="9">
@@ -1615,10 +1657,10 @@
         <v>52</v>
       </c>
       <c r="C9" t="n">
-        <v>6.0</v>
+        <v>2.0</v>
       </c>
       <c r="D9" t="n" s="6">
-        <v>0.75</v>
+        <v>0.6666666666666666</v>
       </c>
     </row>
     <row r="10">
@@ -1632,8 +1674,41 @@
         <v>0.3333333333333333</v>
       </c>
     </row>
+    <row r="11">
+      <c r="B11" t="s" s="3">
+        <v>54</v>
+      </c>
+      <c r="C11" t="n">
+        <v>6.0</v>
+      </c>
+      <c r="D11" t="n" s="6">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="B12" t="s" s="3">
+        <v>55</v>
+      </c>
+      <c r="C12" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="D12" t="n" s="6">
+        <v>0.6666666666666666</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="B13" t="s" s="3">
+        <v>56</v>
+      </c>
+      <c r="C13" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="D13" t="n" s="6">
+        <v>0.3333333333333333</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="B2:D10"/>
+  <autoFilter ref="B2:D13"/>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
* Fixed matched counts in summary layout. * Added the ligreto.strictTypes parameter. * Added the version string. * Added the report name into the assertion exception when the excel files differ.
</commit_message>
<xml_diff>
--- a/tests/data/desired/columnscomparisonreport.xlsx
+++ b/tests/data/desired/columnscomparisonreport.xlsx
@@ -653,7 +653,7 @@
         <v>52</v>
       </c>
       <c r="C9" t="n">
-        <v>2.0</v>
+        <v>4.0</v>
       </c>
       <c r="D9" t="n" s="6">
         <v>0.6666666666666666</v>
@@ -686,7 +686,7 @@
         <v>55</v>
       </c>
       <c r="C12" t="n">
-        <v>2.0</v>
+        <v>4.0</v>
       </c>
       <c r="D12" t="n" s="6">
         <v>0.6666666666666666</v>
@@ -1657,7 +1657,7 @@
         <v>52</v>
       </c>
       <c r="C9" t="n">
-        <v>2.0</v>
+        <v>4.0</v>
       </c>
       <c r="D9" t="n" s="6">
         <v>0.6666666666666666</v>
@@ -1690,7 +1690,7 @@
         <v>55</v>
       </c>
       <c r="C12" t="n">
-        <v>2.0</v>
+        <v>4.0</v>
       </c>
       <c r="D12" t="n" s="6">
         <v>0.6666666666666666</v>

</xml_diff>

<commit_message>
* Bug fixes after major code refactoring.
</commit_message>
<xml_diff>
--- a/tests/data/desired/columnscomparisonreport.xlsx
+++ b/tests/data/desired/columnscomparisonreport.xlsx
@@ -16,6 +16,7 @@
     <sheet name="detailed2" r:id="rId10" sheetId="8"/>
     <sheet name="aggregated2" r:id="rId11" sheetId="9"/>
     <sheet name="summary2" r:id="rId12" sheetId="10"/>
+    <sheet name="nocolumns" r:id="rId13" sheetId="11"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="true">interlaced!$B$2:$I$10</definedName>
@@ -28,12 +29,13 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="true">detailed2!$B$2:$G$26</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="8" hidden="true">aggregated2!$B$2:$H$5</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="9" hidden="true">summary2!$B$2:$D$13</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="10" hidden="true">nocolumns!$B$2:$I$10</definedName>
   </definedNames>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="408" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="452" uniqueCount="57">
   <si>
     <t># of Diffs</t>
   </si>
@@ -709,6 +711,264 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <cols>
+    <col min="2" max="2" width="14.03515625" customWidth="true" bestFit="true"/>
+    <col min="3" max="3" width="7.01171875" customWidth="true" bestFit="true"/>
+    <col min="4" max="4" width="26.10546875" customWidth="true" bestFit="true"/>
+    <col min="5" max="5" width="26.10546875" customWidth="true" bestFit="true"/>
+    <col min="6" max="6" width="25.59765625" customWidth="true" bestFit="true"/>
+    <col min="7" max="7" width="25.59765625" customWidth="true" bestFit="true"/>
+    <col min="8" max="8" width="18.390625" customWidth="true" bestFit="true"/>
+    <col min="9" max="9" width="18.390625" customWidth="true" bestFit="true"/>
+  </cols>
+  <sheetData>
+    <row r="2">
+      <c r="B2" t="s" s="1">
+        <v>0</v>
+      </c>
+      <c r="C2" t="s" s="1">
+        <v>1</v>
+      </c>
+      <c r="D2" t="s" s="1">
+        <v>2</v>
+      </c>
+      <c r="E2" t="s" s="1">
+        <v>5</v>
+      </c>
+      <c r="F2" t="s" s="1">
+        <v>3</v>
+      </c>
+      <c r="G2" t="s" s="1">
+        <v>6</v>
+      </c>
+      <c r="H2" t="s" s="1">
+        <v>4</v>
+      </c>
+      <c r="I2" t="s" s="1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="B3" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C3" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="D3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E3" t="s">
+        <v>21</v>
+      </c>
+      <c r="F3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G3" t="s">
+        <v>22</v>
+      </c>
+      <c r="H3" t="n">
+        <v>11.0</v>
+      </c>
+      <c r="I3" t="n">
+        <v>21.0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="B4" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C4" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="D4" t="s">
+        <v>28</v>
+      </c>
+      <c r="E4" t="s">
+        <v>30</v>
+      </c>
+      <c r="F4" t="s">
+        <v>29</v>
+      </c>
+      <c r="G4" t="s">
+        <v>31</v>
+      </c>
+      <c r="H4" t="n">
+        <v>12.0</v>
+      </c>
+      <c r="I4" t="n">
+        <v>22.0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="B5" t="n" s="2">
+        <v>3.0</v>
+      </c>
+      <c r="C5" t="n" s="2">
+        <v>3.0</v>
+      </c>
+      <c r="D5" t="s">
+        <v>32</v>
+      </c>
+      <c r="E5" t="s">
+        <v>34</v>
+      </c>
+      <c r="F5" t="s">
+        <v>33</v>
+      </c>
+      <c r="G5" t="s">
+        <v>34</v>
+      </c>
+      <c r="H5" t="n">
+        <v>13.0</v>
+      </c>
+      <c r="I5" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="B6" t="n" s="2">
+        <v>3.0</v>
+      </c>
+      <c r="C6" t="n" s="2">
+        <v>4.0</v>
+      </c>
+      <c r="D6" t="s">
+        <v>34</v>
+      </c>
+      <c r="E6" t="s">
+        <v>35</v>
+      </c>
+      <c r="F6" t="s">
+        <v>34</v>
+      </c>
+      <c r="G6" t="s">
+        <v>36</v>
+      </c>
+      <c r="H6" t="s">
+        <v>34</v>
+      </c>
+      <c r="I6" t="n">
+        <v>24.0</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="B7" t="n" s="2">
+        <v>3.0</v>
+      </c>
+      <c r="C7" t="n" s="2">
+        <v>5.0</v>
+      </c>
+      <c r="D7" t="s">
+        <v>37</v>
+      </c>
+      <c r="E7" t="s">
+        <v>34</v>
+      </c>
+      <c r="F7" t="s">
+        <v>38</v>
+      </c>
+      <c r="G7" t="s">
+        <v>34</v>
+      </c>
+      <c r="H7" t="n">
+        <v>15.0</v>
+      </c>
+      <c r="I7" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="B8" t="n" s="2">
+        <v>3.0</v>
+      </c>
+      <c r="C8" t="n" s="2">
+        <v>6.0</v>
+      </c>
+      <c r="D8" t="s">
+        <v>34</v>
+      </c>
+      <c r="E8" t="s">
+        <v>39</v>
+      </c>
+      <c r="F8" t="s">
+        <v>34</v>
+      </c>
+      <c r="G8" t="s">
+        <v>40</v>
+      </c>
+      <c r="H8" t="s">
+        <v>34</v>
+      </c>
+      <c r="I8" t="n">
+        <v>26.0</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="B9" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C9" t="n">
+        <v>7.0</v>
+      </c>
+      <c r="D9" t="s">
+        <v>41</v>
+      </c>
+      <c r="E9" t="s">
+        <v>41</v>
+      </c>
+      <c r="F9" t="s">
+        <v>42</v>
+      </c>
+      <c r="G9" t="s">
+        <v>42</v>
+      </c>
+      <c r="H9" t="n">
+        <v>77.0</v>
+      </c>
+      <c r="I9" t="n">
+        <v>77.0</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="B10" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C10" t="n">
+        <v>8.0</v>
+      </c>
+      <c r="D10" t="s">
+        <v>44</v>
+      </c>
+      <c r="E10" t="s">
+        <v>44</v>
+      </c>
+      <c r="F10" t="s">
+        <v>45</v>
+      </c>
+      <c r="G10" t="s">
+        <v>45</v>
+      </c>
+      <c r="H10" t="n">
+        <v>15.0</v>
+      </c>
+      <c r="I10" t="n">
+        <v>88.0</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="B2:I10"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <dimension ref="A1"/>

</xml_diff>

<commit_message>
* Fixed the problem with wrong order of rows detection. * Nulls are currently always sorted first. * Added the description to header "Value in SRC_DESC" instead of "SRC_DESC" to detailed report.
</commit_message>
<xml_diff>
--- a/tests/data/desired/columnscomparisonreport.xlsx
+++ b/tests/data/desired/columnscomparisonreport.xlsx
@@ -74,10 +74,10 @@
     <t>Column Name</t>
   </si>
   <si>
-    <t>Source1</t>
-  </si>
-  <si>
-    <t>Source2</t>
+    <t>Value in Source1</t>
+  </si>
+  <si>
+    <t>Value in Source2</t>
   </si>
   <si>
     <t>Difference</t>
@@ -588,11 +588,6 @@
     <font>
       <name val="Calibri"/>
       <sz val="11.0"/>
-      <color indexed="8"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
       <b val="true"/>
       <color indexed="23"/>
     </font>
@@ -605,6 +600,11 @@
       <name val="Calibri"/>
       <sz val="11.0"/>
       <color indexed="55"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="8"/>
     </font>
     <font>
       <name val="Calibri"/>
@@ -783,9 +783,9 @@
     <xf numFmtId="0" fontId="62" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
     <xf numFmtId="0" fontId="63" fillId="7" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
     <xf numFmtId="165" fontId="64" fillId="7" borderId="0" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true"/>
-    <xf numFmtId="165" fontId="65" fillId="7" borderId="0" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true"/>
-    <xf numFmtId="0" fontId="66" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="67" fillId="7" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="65" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="66" fillId="7" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="165" fontId="67" fillId="7" borderId="0" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true"/>
     <xf numFmtId="165" fontId="68" fillId="7" borderId="0" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true"/>
     <xf numFmtId="0" fontId="69" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
     <xf numFmtId="165" fontId="70" fillId="7" borderId="0" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true"/>
@@ -1069,8 +1069,8 @@
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
     <col min="2" max="2" width="35.66015625" customWidth="true" bestFit="true"/>
-    <col min="3" max="3" width="10.32421875" customWidth="true" bestFit="true"/>
-    <col min="4" max="4" width="12.4609375" customWidth="true" bestFit="true"/>
+    <col min="3" max="3" width="10.328125" customWidth="true" bestFit="true"/>
+    <col min="4" max="4" width="12.46484375" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="2">
@@ -1268,10 +1268,10 @@
       <c r="E3" t="s" s="58">
         <v>20</v>
       </c>
-      <c r="F3" t="n">
+      <c r="F3" t="n" s="58">
         <v>11.0</v>
       </c>
-      <c r="G3" t="n">
+      <c r="G3" t="n" s="58">
         <v>21.0</v>
       </c>
       <c r="H3" t="s" s="59">
@@ -1294,10 +1294,10 @@
       <c r="E4" t="s" s="58">
         <v>29</v>
       </c>
-      <c r="F4" t="n">
+      <c r="F4" t="n" s="58">
         <v>12.0</v>
       </c>
-      <c r="G4" t="n">
+      <c r="G4" t="n" s="58">
         <v>22.0</v>
       </c>
       <c r="H4" t="s" s="59">
@@ -1450,10 +1450,10 @@
       <c r="E10" t="s">
         <v>44</v>
       </c>
-      <c r="F10" t="n">
+      <c r="F10" t="n" s="58">
         <v>15.0</v>
       </c>
-      <c r="G10" t="n">
+      <c r="G10" t="n" s="58">
         <v>88.0</v>
       </c>
       <c r="H10" t="s" s="59">
@@ -1523,13 +1523,13 @@
       <c r="D3" t="s" s="60">
         <v>19</v>
       </c>
-      <c r="E3" t="n">
+      <c r="E3" t="n" s="60">
         <v>11.0</v>
       </c>
       <c r="F3" t="s" s="60">
         <v>20</v>
       </c>
-      <c r="G3" t="n">
+      <c r="G3" t="n" s="60">
         <v>21.0</v>
       </c>
       <c r="H3" t="s" s="61">
@@ -1549,13 +1549,13 @@
       <c r="D4" t="s" s="60">
         <v>28</v>
       </c>
-      <c r="E4" t="n">
+      <c r="E4" t="n" s="60">
         <v>12.0</v>
       </c>
       <c r="F4" t="s" s="60">
         <v>29</v>
       </c>
-      <c r="G4" t="n">
+      <c r="G4" t="n" s="60">
         <v>22.0</v>
       </c>
       <c r="H4" t="s" s="61">
@@ -1705,13 +1705,13 @@
       <c r="D10" t="s">
         <v>44</v>
       </c>
-      <c r="E10" t="n">
+      <c r="E10" t="n" s="60">
         <v>15.0</v>
       </c>
       <c r="F10" t="s">
         <v>44</v>
       </c>
-      <c r="G10" t="n">
+      <c r="G10" t="n" s="60">
         <v>88.0</v>
       </c>
       <c r="H10" t="s" s="61">
@@ -1737,9 +1737,9 @@
   <cols>
     <col min="2" max="2" width="18.234375" customWidth="true" bestFit="true"/>
     <col min="3" max="3" width="7.01171875" customWidth="true" bestFit="true"/>
-    <col min="4" max="4" width="17.59375" customWidth="true" bestFit="true"/>
-    <col min="5" max="5" width="17.59375" customWidth="true" bestFit="true"/>
-    <col min="6" max="6" width="14.75390625" customWidth="true" bestFit="true"/>
+    <col min="4" max="4" width="20.8515625" customWidth="true" bestFit="true"/>
+    <col min="5" max="5" width="20.8515625" customWidth="true" bestFit="true"/>
+    <col min="6" max="6" width="14.7578125" customWidth="true" bestFit="true"/>
     <col min="7" max="7" width="13.7109375" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
@@ -1790,36 +1790,36 @@
       <c r="C4" t="n">
         <v>1.0</v>
       </c>
-      <c r="D4" t="n">
+      <c r="D4" t="n" s="63">
         <v>11.0</v>
       </c>
-      <c r="E4" t="n">
+      <c r="E4" t="n" s="63">
         <v>21.0</v>
       </c>
-      <c r="F4" t="n">
+      <c r="F4" t="n" s="63">
         <v>10.0</v>
       </c>
-      <c r="G4" t="n" s="65">
+      <c r="G4" t="n" s="64">
         <v>0.9090909090909091</v>
       </c>
     </row>
     <row r="5">
-      <c r="B5" t="s" s="66">
+      <c r="B5" t="s" s="65">
         <v>26</v>
       </c>
-      <c r="C5" t="n" s="67">
+      <c r="C5" t="n" s="66">
         <v>1.0</v>
       </c>
-      <c r="D5" t="s" s="67">
+      <c r="D5" t="s" s="66">
         <v>21</v>
       </c>
-      <c r="E5" t="s" s="67">
+      <c r="E5" t="s" s="66">
         <v>22</v>
       </c>
-      <c r="F5" t="s" s="67">
+      <c r="F5" t="s" s="66">
         <v>24</v>
       </c>
-      <c r="G5" t="s" s="68">
+      <c r="G5" t="s" s="67">
         <v>25</v>
       </c>
     </row>
@@ -1850,36 +1850,36 @@
       <c r="C7" t="n">
         <v>2.0</v>
       </c>
-      <c r="D7" t="n">
+      <c r="D7" t="n" s="63">
         <v>12.0</v>
       </c>
-      <c r="E7" t="n">
+      <c r="E7" t="n" s="63">
         <v>22.0</v>
       </c>
-      <c r="F7" t="n">
+      <c r="F7" t="n" s="63">
         <v>10.0</v>
       </c>
-      <c r="G7" t="n" s="65">
+      <c r="G7" t="n" s="64">
         <v>0.8333333333333334</v>
       </c>
     </row>
     <row r="8">
-      <c r="B8" t="s" s="66">
+      <c r="B8" t="s" s="65">
         <v>26</v>
       </c>
-      <c r="C8" t="n" s="67">
+      <c r="C8" t="n" s="66">
         <v>2.0</v>
       </c>
-      <c r="D8" t="s" s="67">
+      <c r="D8" t="s" s="66">
         <v>30</v>
       </c>
-      <c r="E8" t="s" s="67">
+      <c r="E8" t="s" s="66">
         <v>31</v>
       </c>
-      <c r="F8" t="s" s="67">
+      <c r="F8" t="s" s="66">
         <v>24</v>
       </c>
-      <c r="G8" t="s" s="68">
+      <c r="G8" t="s" s="67">
         <v>25</v>
       </c>
     </row>
@@ -1921,19 +1921,19 @@
       </c>
     </row>
     <row r="11">
-      <c r="B11" t="s" s="66">
+      <c r="B11" t="s" s="65">
         <v>26</v>
       </c>
-      <c r="C11" t="n" s="67">
+      <c r="C11" t="n" s="66">
         <v>3.0</v>
       </c>
-      <c r="D11" t="s" s="67">
+      <c r="D11" t="s" s="66">
         <v>34</v>
       </c>
-      <c r="E11" t="s" s="67">
-        <v>33</v>
-      </c>
-      <c r="F11" t="s" s="67">
+      <c r="E11" t="s" s="66">
+        <v>33</v>
+      </c>
+      <c r="F11" t="s" s="66">
         <v>24</v>
       </c>
     </row>
@@ -1975,19 +1975,19 @@
       </c>
     </row>
     <row r="14">
-      <c r="B14" t="s" s="66">
+      <c r="B14" t="s" s="65">
         <v>26</v>
       </c>
-      <c r="C14" t="n" s="67">
+      <c r="C14" t="n" s="66">
         <v>4.0</v>
       </c>
-      <c r="D14" t="s" s="67">
-        <v>33</v>
-      </c>
-      <c r="E14" t="s" s="67">
+      <c r="D14" t="s" s="66">
+        <v>33</v>
+      </c>
+      <c r="E14" t="s" s="66">
         <v>36</v>
       </c>
-      <c r="F14" t="s" s="67">
+      <c r="F14" t="s" s="66">
         <v>24</v>
       </c>
     </row>
@@ -2029,19 +2029,19 @@
       </c>
     </row>
     <row r="17">
-      <c r="B17" t="s" s="66">
+      <c r="B17" t="s" s="65">
         <v>26</v>
       </c>
-      <c r="C17" t="n" s="67">
+      <c r="C17" t="n" s="66">
         <v>5.0</v>
       </c>
-      <c r="D17" t="s" s="67">
+      <c r="D17" t="s" s="66">
         <v>38</v>
       </c>
-      <c r="E17" t="s" s="67">
-        <v>33</v>
-      </c>
-      <c r="F17" t="s" s="67">
+      <c r="E17" t="s" s="66">
+        <v>33</v>
+      </c>
+      <c r="F17" t="s" s="66">
         <v>24</v>
       </c>
     </row>
@@ -2083,19 +2083,19 @@
       </c>
     </row>
     <row r="20">
-      <c r="B20" t="s" s="66">
+      <c r="B20" t="s" s="65">
         <v>26</v>
       </c>
-      <c r="C20" t="n" s="67">
+      <c r="C20" t="n" s="66">
         <v>6.0</v>
       </c>
-      <c r="D20" t="s" s="67">
-        <v>33</v>
-      </c>
-      <c r="E20" t="s" s="67">
+      <c r="D20" t="s" s="66">
+        <v>33</v>
+      </c>
+      <c r="E20" t="s" s="66">
         <v>40</v>
       </c>
-      <c r="F20" t="s" s="67">
+      <c r="F20" t="s" s="66">
         <v>24</v>
       </c>
     </row>
@@ -2115,7 +2115,7 @@
       <c r="F21" t="s">
         <v>43</v>
       </c>
-      <c r="G21" t="s" s="65">
+      <c r="G21" t="s" s="68">
         <v>25</v>
       </c>
     </row>
@@ -2135,27 +2135,27 @@
       <c r="F22" t="s">
         <v>43</v>
       </c>
-      <c r="G22" t="s" s="65">
+      <c r="G22" t="s" s="68">
         <v>25</v>
       </c>
     </row>
     <row r="23">
-      <c r="B23" t="s" s="66">
+      <c r="B23" t="s" s="65">
         <v>26</v>
       </c>
-      <c r="C23" t="n" s="67">
+      <c r="C23" t="n" s="66">
         <v>7.0</v>
       </c>
-      <c r="D23" t="s" s="67">
+      <c r="D23" t="s" s="66">
         <v>42</v>
       </c>
-      <c r="E23" t="s" s="67">
+      <c r="E23" t="s" s="66">
         <v>42</v>
       </c>
-      <c r="F23" t="s" s="67">
+      <c r="F23" t="s" s="66">
         <v>43</v>
       </c>
-      <c r="G23" t="s" s="68">
+      <c r="G23" t="s" s="67">
         <v>25</v>
       </c>
     </row>
@@ -2175,7 +2175,7 @@
       <c r="F24" t="s">
         <v>43</v>
       </c>
-      <c r="G24" t="s" s="65">
+      <c r="G24" t="s" s="68">
         <v>25</v>
       </c>
     </row>
@@ -2186,36 +2186,36 @@
       <c r="C25" t="n">
         <v>8.0</v>
       </c>
-      <c r="D25" t="n">
+      <c r="D25" t="n" s="63">
         <v>15.0</v>
       </c>
-      <c r="E25" t="n">
+      <c r="E25" t="n" s="63">
         <v>88.0</v>
       </c>
-      <c r="F25" t="n">
+      <c r="F25" t="n" s="63">
         <v>73.0</v>
       </c>
-      <c r="G25" t="n" s="65">
+      <c r="G25" t="n" s="64">
         <v>4.866666666666666</v>
       </c>
     </row>
     <row r="26">
-      <c r="B26" t="s" s="66">
+      <c r="B26" t="s" s="65">
         <v>26</v>
       </c>
-      <c r="C26" t="n" s="67">
+      <c r="C26" t="n" s="66">
         <v>8.0</v>
       </c>
-      <c r="D26" t="s" s="67">
+      <c r="D26" t="s" s="66">
         <v>45</v>
       </c>
-      <c r="E26" t="s" s="67">
+      <c r="E26" t="s" s="66">
         <v>45</v>
       </c>
-      <c r="F26" t="s" s="67">
+      <c r="F26" t="s" s="66">
         <v>43</v>
       </c>
-      <c r="G26" t="s" s="68">
+      <c r="G26" t="s" s="67">
         <v>25</v>
       </c>
     </row>
@@ -2235,9 +2235,9 @@
   <cols>
     <col min="2" max="2" width="18.234375" customWidth="true" bestFit="true"/>
     <col min="3" max="3" width="14.03515625" customWidth="true" bestFit="true"/>
-    <col min="4" max="4" width="17.546875" customWidth="true" bestFit="true"/>
-    <col min="5" max="5" width="22.87109375" customWidth="true" bestFit="true"/>
-    <col min="6" max="6" width="14.75390625" customWidth="true" bestFit="true"/>
+    <col min="4" max="4" width="17.55078125" customWidth="true" bestFit="true"/>
+    <col min="5" max="5" width="22.875" customWidth="true" bestFit="true"/>
+    <col min="6" max="6" width="14.7578125" customWidth="true" bestFit="true"/>
     <col min="7" max="7" width="14.484375" customWidth="true" bestFit="true"/>
     <col min="8" max="8" width="15.78515625" customWidth="true" bestFit="true"/>
   </cols>
@@ -2331,8 +2331,8 @@
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
     <col min="2" max="2" width="35.66015625" customWidth="true" bestFit="true"/>
-    <col min="3" max="3" width="10.32421875" customWidth="true" bestFit="true"/>
-    <col min="4" max="4" width="12.4609375" customWidth="true" bestFit="true"/>
+    <col min="3" max="3" width="10.328125" customWidth="true" bestFit="true"/>
+    <col min="4" max="4" width="12.46484375" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="2">
@@ -2999,9 +2999,9 @@
   <cols>
     <col min="2" max="2" width="18.234375" customWidth="true" bestFit="true"/>
     <col min="3" max="3" width="7.01171875" customWidth="true" bestFit="true"/>
-    <col min="4" max="4" width="17.59375" customWidth="true" bestFit="true"/>
-    <col min="5" max="5" width="17.59375" customWidth="true" bestFit="true"/>
-    <col min="6" max="6" width="14.75390625" customWidth="true" bestFit="true"/>
+    <col min="4" max="4" width="20.8515625" customWidth="true" bestFit="true"/>
+    <col min="5" max="5" width="20.8515625" customWidth="true" bestFit="true"/>
+    <col min="6" max="6" width="14.7578125" customWidth="true" bestFit="true"/>
     <col min="7" max="7" width="13.7109375" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
@@ -3497,9 +3497,9 @@
   <cols>
     <col min="2" max="2" width="18.234375" customWidth="true" bestFit="true"/>
     <col min="3" max="3" width="14.03515625" customWidth="true" bestFit="true"/>
-    <col min="4" max="4" width="17.546875" customWidth="true" bestFit="true"/>
-    <col min="5" max="5" width="22.87109375" customWidth="true" bestFit="true"/>
-    <col min="6" max="6" width="14.75390625" customWidth="true" bestFit="true"/>
+    <col min="4" max="4" width="17.55078125" customWidth="true" bestFit="true"/>
+    <col min="5" max="5" width="22.875" customWidth="true" bestFit="true"/>
+    <col min="6" max="6" width="14.7578125" customWidth="true" bestFit="true"/>
     <col min="7" max="7" width="14.484375" customWidth="true" bestFit="true"/>
     <col min="8" max="8" width="15.78515625" customWidth="true" bestFit="true"/>
   </cols>
@@ -3593,8 +3593,8 @@
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
     <col min="2" max="2" width="35.66015625" customWidth="true" bestFit="true"/>
-    <col min="3" max="3" width="10.32421875" customWidth="true" bestFit="true"/>
-    <col min="4" max="4" width="12.4609375" customWidth="true" bestFit="true"/>
+    <col min="3" max="3" width="10.328125" customWidth="true" bestFit="true"/>
+    <col min="4" max="4" width="12.46484375" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="2">
@@ -4261,9 +4261,9 @@
   <cols>
     <col min="2" max="2" width="18.234375" customWidth="true" bestFit="true"/>
     <col min="3" max="3" width="7.01171875" customWidth="true" bestFit="true"/>
-    <col min="4" max="4" width="17.59375" customWidth="true" bestFit="true"/>
-    <col min="5" max="5" width="17.59375" customWidth="true" bestFit="true"/>
-    <col min="6" max="6" width="14.75390625" customWidth="true" bestFit="true"/>
+    <col min="4" max="4" width="20.8515625" customWidth="true" bestFit="true"/>
+    <col min="5" max="5" width="20.8515625" customWidth="true" bestFit="true"/>
+    <col min="6" max="6" width="14.7578125" customWidth="true" bestFit="true"/>
     <col min="7" max="7" width="13.7109375" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
@@ -4759,9 +4759,9 @@
   <cols>
     <col min="2" max="2" width="18.234375" customWidth="true" bestFit="true"/>
     <col min="3" max="3" width="14.03515625" customWidth="true" bestFit="true"/>
-    <col min="4" max="4" width="17.546875" customWidth="true" bestFit="true"/>
-    <col min="5" max="5" width="22.87109375" customWidth="true" bestFit="true"/>
-    <col min="6" max="6" width="14.75390625" customWidth="true" bestFit="true"/>
+    <col min="4" max="4" width="17.55078125" customWidth="true" bestFit="true"/>
+    <col min="5" max="5" width="22.875" customWidth="true" bestFit="true"/>
+    <col min="6" max="6" width="14.7578125" customWidth="true" bestFit="true"/>
     <col min="7" max="7" width="14.484375" customWidth="true" bestFit="true"/>
     <col min="8" max="8" width="15.78515625" customWidth="true" bestFit="true"/>
   </cols>

</xml_diff>